<commit_message>
bugfix, assembler and counter assembly added
</commit_message>
<xml_diff>
--- a/instructions_control_details.xlsx
+++ b/instructions_control_details.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Instruction Set" sheetId="1" state="visible" r:id="rId2"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="101">
   <si>
     <t xml:space="preserve">Instruction</t>
   </si>
@@ -259,6 +259,10 @@
 stops clock</t>
   </si>
   <si>
+    <t xml:space="preserve">INCREMENT &amp; MEMORY IGNORE State
+Increment PC and ignore memory value, used for conditional jumps when conditions didn’t met</t>
+  </si>
+  <si>
     <t xml:space="preserve">State Numbers</t>
   </si>
   <si>
@@ -298,7 +302,7 @@
     <t xml:space="preserve">1, 2, 1, 12, 3</t>
   </si>
   <si>
-    <t xml:space="preserve">1, 2, 1, [12 if met], 3</t>
+    <t xml:space="preserve">1, 2, 1, [12 if met 14 otherwise], 3</t>
   </si>
   <si>
     <t xml:space="preserve">Carry Flag</t>
@@ -822,8 +826,8 @@
   </sheetPr>
   <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D15" activeCellId="0" sqref="D15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C15" activeCellId="0" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1366,8 +1370,8 @@
   </sheetPr>
   <dimension ref="A1:U33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="K1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="T2" activeCellId="0" sqref="T2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1950,9 +1954,13 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="13"/>
-      <c r="B15" s="17"/>
+    <row r="15" customFormat="false" ht="46.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="13" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="17" t="s">
+        <v>68</v>
+      </c>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
       <c r="E15" s="15"/>
@@ -1967,11 +1975,19 @@
       <c r="N15" s="15"/>
       <c r="O15" s="15"/>
       <c r="P15" s="15"/>
-      <c r="Q15" s="15"/>
+      <c r="Q15" s="15" t="n">
+        <v>1</v>
+      </c>
       <c r="R15" s="15"/>
       <c r="S15" s="15"/>
-      <c r="T15" s="16"/>
-      <c r="U15" s="16"/>
+      <c r="T15" s="16" t="str">
+        <f aca="false">_xlfn.CONCAT(IF(C15=1, 1, 0), IF(D15=1, 1, 0), IF(E15=1, 1, 0), IF(F15=1, 1, 0), IF(G15=1, 1, 0), IF(H15=1, 1, 0), IF(I15=1, 1, 0), IF(J15=1, 1, 0), IF(K15=1, 1, 0), IF(L15=1, 1, 0), IF(M15=1, 1, 0), IF(N15=1, 1, 0), IF(O15=1, 1, 0), IF(P15=1, 1, 0), IF(Q15=1, 1, 0), IF(R15=1, 1, 0), IF(S15=1, 1, 0))</f>
+        <v>00000000000000100</v>
+      </c>
+      <c r="U15" s="16" t="str">
+        <f aca="false">_xlfn.BASE(_xlfn.DECIMAL(T15,2),16)</f>
+        <v>4</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="13"/>
@@ -2406,13 +2422,13 @@
   <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="36.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="56.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="23.03"/>
@@ -2423,7 +2439,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2431,7 +2447,7 @@
         <v>5</v>
       </c>
       <c r="B2" s="20" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2439,7 +2455,7 @@
         <v>8</v>
       </c>
       <c r="B3" s="20" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2447,7 +2463,7 @@
         <v>10</v>
       </c>
       <c r="B4" s="20" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2455,7 +2471,7 @@
         <v>12</v>
       </c>
       <c r="B5" s="20" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2463,7 +2479,7 @@
         <v>14</v>
       </c>
       <c r="B6" s="20" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2471,7 +2487,7 @@
         <v>16</v>
       </c>
       <c r="B7" s="20" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2479,7 +2495,7 @@
         <v>18</v>
       </c>
       <c r="B8" s="20" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2487,7 +2503,7 @@
         <v>20</v>
       </c>
       <c r="B9" s="20" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2495,7 +2511,7 @@
         <v>22</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2503,7 +2519,7 @@
         <v>24</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2511,7 +2527,7 @@
         <v>26</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2519,7 +2535,7 @@
         <v>28</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2527,7 +2543,7 @@
         <v>30</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="22.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2535,7 +2551,7 @@
         <v>32</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
@@ -2556,8 +2572,8 @@
   </sheetPr>
   <dimension ref="A1:F299"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AO70" activeCellId="0" sqref="AO70"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H56" activeCellId="0" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2575,28 +2591,28 @@
         <v>2</v>
       </c>
       <c r="B1" s="23" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D1" s="24" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="E1" s="25"/>
       <c r="F1" s="26" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="27" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B2" s="27" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C2" s="27" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D2" s="27" t="n">
         <v>0</v>
@@ -2608,13 +2624,13 @@
     </row>
     <row r="3" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="27" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B3" s="27" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C3" s="27" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D3" s="27" t="n">
         <v>1</v>
@@ -2637,10 +2653,10 @@
         <v>6</v>
       </c>
       <c r="B5" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C5" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D5" s="29" t="n">
         <v>2</v>
@@ -2660,13 +2676,13 @@
     </row>
     <row r="7" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="29" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B7" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C7" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D7" s="29" t="n">
         <v>2</v>
@@ -2686,13 +2702,13 @@
     </row>
     <row r="9" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="29" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B9" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C9" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D9" s="29" t="n">
         <v>2</v>
@@ -2704,13 +2720,13 @@
     </row>
     <row r="10" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="29" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B10" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C10" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D10" s="29" t="n">
         <v>3</v>
@@ -2722,13 +2738,13 @@
     </row>
     <row r="11" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="29" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B11" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C11" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D11" s="29" t="n">
         <v>4</v>
@@ -2748,13 +2764,13 @@
     </row>
     <row r="13" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="29" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B13" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C13" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D13" s="29" t="n">
         <v>2</v>
@@ -2766,13 +2782,13 @@
     </row>
     <row r="14" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="29" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B14" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C14" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D14" s="29" t="n">
         <v>3</v>
@@ -2784,13 +2800,13 @@
     </row>
     <row r="15" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="29" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B15" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C15" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D15" s="29" t="n">
         <v>4</v>
@@ -2802,13 +2818,13 @@
     </row>
     <row r="16" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="29" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D16" s="29" t="n">
         <v>5</v>
@@ -2828,13 +2844,13 @@
     </row>
     <row r="18" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="29" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B18" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C18" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D18" s="29" t="n">
         <v>2</v>
@@ -2846,13 +2862,13 @@
     </row>
     <row r="19" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="29" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B19" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C19" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D19" s="29" t="n">
         <v>3</v>
@@ -2864,13 +2880,13 @@
     </row>
     <row r="20" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="29" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B20" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C20" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D20" s="29" t="n">
         <v>4</v>
@@ -2882,13 +2898,13 @@
     </row>
     <row r="21" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="29" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B21" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C21" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D21" s="29" t="n">
         <v>5</v>
@@ -2908,13 +2924,13 @@
     </row>
     <row r="23" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="29" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B23" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C23" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D23" s="29" t="n">
         <v>2</v>
@@ -2926,13 +2942,13 @@
     </row>
     <row r="24" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="29" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B24" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C24" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D24" s="29" t="n">
         <v>3</v>
@@ -2944,13 +2960,13 @@
     </row>
     <row r="25" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="29" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B25" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C25" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D25" s="29" t="n">
         <v>4</v>
@@ -2970,13 +2986,13 @@
     </row>
     <row r="27" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="29" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B27" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C27" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D27" s="29" t="n">
         <v>2</v>
@@ -2988,13 +3004,13 @@
     </row>
     <row r="28" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="29" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B28" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C28" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D28" s="29" t="n">
         <v>3</v>
@@ -3006,13 +3022,13 @@
     </row>
     <row r="29" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="29" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B29" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C29" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D29" s="29" t="n">
         <v>4</v>
@@ -3024,13 +3040,13 @@
     </row>
     <row r="30" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="29" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B30" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C30" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D30" s="29" t="n">
         <v>5</v>
@@ -3050,13 +3066,13 @@
     </row>
     <row r="32" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="29" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B32" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C32" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D32" s="29" t="n">
         <v>2</v>
@@ -3068,13 +3084,13 @@
     </row>
     <row r="33" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="29" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B33" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C33" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D33" s="29" t="n">
         <v>3</v>
@@ -3086,13 +3102,13 @@
     </row>
     <row r="34" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="29" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B34" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C34" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D34" s="29" t="n">
         <v>4</v>
@@ -3104,13 +3120,13 @@
     </row>
     <row r="35" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="29" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B35" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C35" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D35" s="29" t="n">
         <v>5</v>
@@ -3130,13 +3146,13 @@
     </row>
     <row r="37" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="29" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B37" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C37" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D37" s="29" t="n">
         <v>2</v>
@@ -3148,13 +3164,13 @@
     </row>
     <row r="38" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="29" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B38" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C38" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D38" s="29" t="n">
         <v>3</v>
@@ -3174,13 +3190,13 @@
     </row>
     <row r="40" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="29" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B40" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C40" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D40" s="29" t="n">
         <v>2</v>
@@ -3192,13 +3208,13 @@
     </row>
     <row r="41" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="29" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B41" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C41" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D41" s="29" t="n">
         <v>3</v>
@@ -3218,13 +3234,13 @@
     </row>
     <row r="43" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="29" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B43" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C43" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D43" s="29" t="n">
         <v>2</v>
@@ -3236,13 +3252,13 @@
     </row>
     <row r="44" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="29" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B44" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C44" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D44" s="29" t="n">
         <v>3</v>
@@ -3262,13 +3278,13 @@
     </row>
     <row r="46" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="29" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B46" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C46" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D46" s="29" t="n">
         <v>2</v>
@@ -3280,13 +3296,13 @@
     </row>
     <row r="47" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="29" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B47" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C47" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D47" s="29" t="n">
         <v>3</v>
@@ -3298,13 +3314,13 @@
     </row>
     <row r="48" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="29" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B48" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C48" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D48" s="29" t="n">
         <v>4</v>
@@ -3324,13 +3340,13 @@
     </row>
     <row r="50" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="29" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B50" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C50" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D50" s="29" t="n">
         <v>2</v>
@@ -3342,10 +3358,10 @@
     </row>
     <row r="51" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="29" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B51" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C51" s="29" t="n">
         <v>1</v>
@@ -3360,10 +3376,10 @@
     </row>
     <row r="52" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="29" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B52" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C52" s="29" t="n">
         <v>0</v>
@@ -3373,18 +3389,18 @@
       </c>
       <c r="E52" s="28"/>
       <c r="F52" s="29" t="n">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="29" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B53" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C53" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D53" s="29" t="n">
         <v>4</v>
@@ -3404,13 +3420,13 @@
     </row>
     <row r="55" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="29" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B55" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C55" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D55" s="29" t="n">
         <v>2</v>
@@ -3422,13 +3438,13 @@
     </row>
     <row r="56" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="29" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B56" s="29" t="n">
         <v>1</v>
       </c>
       <c r="C56" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D56" s="29" t="n">
         <v>3</v>
@@ -3440,31 +3456,31 @@
     </row>
     <row r="57" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="29" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B57" s="29" t="n">
         <v>0</v>
       </c>
       <c r="C57" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D57" s="29" t="n">
         <v>3</v>
       </c>
       <c r="E57" s="28"/>
       <c r="F57" s="29" t="n">
-        <v>3</v>
+        <v>14</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="29" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B58" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C58" s="29" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D58" s="29" t="n">
         <v>4</v>

</xml_diff>

<commit_message>
bugfixes, project file structure improvement
</commit_message>
<xml_diff>
--- a/instructions_control_details.xlsx
+++ b/instructions_control_details.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Instruction Set" sheetId="1" state="visible" r:id="rId2"/>
@@ -219,8 +219,8 @@
 end instruction</t>
   </si>
   <si>
-    <t xml:space="preserve">INCREMENT &amp; MEMORY – MAR LATCH State
-increment PC and put memory content to MAR</t>
+    <t xml:space="preserve">MEMORY – MAR LATCH State
+put memory content to MAR</t>
   </si>
   <si>
     <t xml:space="preserve">INCREMENT &amp; MEMORY – A LATCH State
@@ -231,12 +231,12 @@
 increment PC and put memory content to B register</t>
   </si>
   <si>
-    <t xml:space="preserve">A OUT - MEMORY WRITE State
-put A register content to memory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B OUT - MEMORY WRITE State
-put B register content to memory</t>
+    <t xml:space="preserve">INCREMENT &amp; A OUT - MEMORY WRITE State
+increment PC and put A register content to memory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">INCREMENT &amp; B OUT - MEMORY WRITE State
+increment PC and put B register content to memory</t>
   </si>
   <si>
     <t xml:space="preserve">ALU OUT - A &amp; FLAGS LATCH State
@@ -1370,8 +1370,8 @@
   </sheetPr>
   <dimension ref="A1:U33"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1599,18 +1599,16 @@
         <v>1</v>
       </c>
       <c r="P5" s="15"/>
-      <c r="Q5" s="15" t="n">
-        <v>1</v>
-      </c>
+      <c r="Q5" s="15"/>
       <c r="R5" s="15"/>
       <c r="S5" s="15"/>
       <c r="T5" s="16" t="str">
         <f aca="false">_xlfn.CONCAT(IF(C5=1, 1, 0), IF(D5=1, 1, 0), IF(E5=1, 1, 0), IF(F5=1, 1, 0), IF(G5=1, 1, 0), IF(H5=1, 1, 0), IF(I5=1, 1, 0), IF(J5=1, 1, 0), IF(K5=1, 1, 0), IF(L5=1, 1, 0), IF(M5=1, 1, 0), IF(N5=1, 1, 0), IF(O5=1, 1, 0), IF(P5=1, 1, 0), IF(Q5=1, 1, 0), IF(R5=1, 1, 0), IF(S5=1, 1, 0))</f>
-        <v>00000000000110100</v>
+        <v>00000000000110000</v>
       </c>
       <c r="U5" s="16" t="str">
         <f aca="false">_xlfn.BASE(_xlfn.DECIMAL(T5,2),16)</f>
-        <v>34</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="33.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1716,16 +1714,18 @@
       <c r="N8" s="15"/>
       <c r="O8" s="15"/>
       <c r="P8" s="15"/>
-      <c r="Q8" s="15"/>
+      <c r="Q8" s="15" t="n">
+        <v>1</v>
+      </c>
       <c r="R8" s="15"/>
       <c r="S8" s="15"/>
       <c r="T8" s="16" t="str">
         <f aca="false">_xlfn.CONCAT(IF(C8=1, 1, 0), IF(D8=1, 1, 0), IF(E8=1, 1, 0), IF(F8=1, 1, 0), IF(G8=1, 1, 0), IF(H8=1, 1, 0), IF(I8=1, 1, 0), IF(J8=1, 1, 0), IF(K8=1, 1, 0), IF(L8=1, 1, 0), IF(M8=1, 1, 0), IF(N8=1, 1, 0), IF(O8=1, 1, 0), IF(P8=1, 1, 0), IF(Q8=1, 1, 0), IF(R8=1, 1, 0), IF(S8=1, 1, 0))</f>
-        <v>00000001001000000</v>
+        <v>00000001001000100</v>
       </c>
       <c r="U8" s="16" t="str">
         <f aca="false">_xlfn.BASE(_xlfn.DECIMAL(T8,2),16)</f>
-        <v>240</v>
+        <v>244</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="36.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1753,16 +1753,18 @@
       <c r="N9" s="15"/>
       <c r="O9" s="15"/>
       <c r="P9" s="15"/>
-      <c r="Q9" s="15"/>
+      <c r="Q9" s="15" t="n">
+        <v>1</v>
+      </c>
       <c r="R9" s="15"/>
       <c r="S9" s="15"/>
       <c r="T9" s="16" t="str">
         <f aca="false">_xlfn.CONCAT(IF(C9=1, 1, 0), IF(D9=1, 1, 0), IF(E9=1, 1, 0), IF(F9=1, 1, 0), IF(G9=1, 1, 0), IF(H9=1, 1, 0), IF(I9=1, 1, 0), IF(J9=1, 1, 0), IF(K9=1, 1, 0), IF(L9=1, 1, 0), IF(M9=1, 1, 0), IF(N9=1, 1, 0), IF(O9=1, 1, 0), IF(P9=1, 1, 0), IF(Q9=1, 1, 0), IF(R9=1, 1, 0), IF(S9=1, 1, 0))</f>
-        <v>00000100001000000</v>
+        <v>00000100001000100</v>
       </c>
       <c r="U9" s="16" t="str">
         <f aca="false">_xlfn.BASE(_xlfn.DECIMAL(T9,2),16)</f>
-        <v>840</v>
+        <v>844</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="37.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2421,8 +2423,8 @@
   </sheetPr>
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2572,8 +2574,8 @@
   </sheetPr>
   <dimension ref="A1:F299"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H56" activeCellId="0" sqref="H56"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A26" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I58" activeCellId="0" sqref="I58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>